<commit_message>
Finalized UGA PhD Application Materials
</commit_message>
<xml_diff>
--- a/Hammerton CV/cv_data.xlsx
+++ b/Hammerton CV/cv_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="117">
   <si>
     <t>section</t>
   </si>
@@ -49,7 +49,10 @@
     <t>Athens, GA</t>
   </si>
   <si>
-    <t>University of Georgia (Current)</t>
+    <t>University of Georgia</t>
+  </si>
+  <si>
+    <t>Present</t>
   </si>
   <si>
     <t xml:space="preserve">BS, Health Science </t>
@@ -85,16 +88,13 @@
     <t>Preterm birth and environmental exposures: Systematic review (In Progress)</t>
   </si>
   <si>
-    <t>University of Georgia</t>
-  </si>
-  <si>
     <t>Research Assisantship, Dr. Jose Cordero</t>
   </si>
   <si>
     <t>Prenatal exposure to flame retardants and adverse pregnancy outcomes: A systematic review (In Progress)</t>
   </si>
   <si>
-    <t>Contributor, Co-Author</t>
+    <t>Co-Author</t>
   </si>
   <si>
     <t>certs</t>
@@ -160,7 +160,7 @@
     <t>Communication</t>
   </si>
   <si>
-    <t>Participated in clinical, research, and private groups requiring large amounts of communication and collaboration, building experience in healthy and efficient communication skills</t>
+    <t>Experience in clinical, research, and private groups requiring large amounts of collaboration</t>
   </si>
   <si>
     <t>Health Education</t>
@@ -184,7 +184,7 @@
     <t xml:space="preserve">University of Georgia, Department of Epidemiology &amp; Biostatistics </t>
   </si>
   <si>
-    <t>Assist in administrative departmental tasks, faculty retreats/meeting planning, and department event planning. Create and maintain spreadsheets on department classes, students, etc. Develop presentation materials and assist in orientation. Generate documents with information on degree programs, Graduate School processes, etc. Participated in research with Dr. Jose Cordero, planning and implementing a systematic reivew of environmental exposures and preterm birth</t>
+    <t>Assist in administrative departmental tasks, faculty retreats/meeting planning, and department event planning. Create and maintain spreadsheets on department classes, students, etc. Develop presentation materials and assist in orientation. Generate documents with information on degree programs, Graduate School processes, etc. Participate in research with Dr. Jose Cordero, planning and implementing a systematic review of environmental exposures and preterm birth.</t>
   </si>
   <si>
     <t xml:space="preserve">Instuctor, Assistant Manager </t>
@@ -193,7 +193,7 @@
     <t>ILoveKickboxing</t>
   </si>
   <si>
-    <t>Promoted to assistant manager after 9 months of employment. Responsible for personal health promotion and education for members, instructing group fitness classes, data management. with membership and point-of-sale systems. Integral part in data transfer when changing systems.</t>
+    <t>Promoted to assistant manager after 9 months of employment. Responsible for personal health promotion and education for members, instructing group fitness classes, data management with membership and point-of-sale systems. Integral part in data transfer when changing systems.</t>
   </si>
   <si>
     <t>Licensed Vocational Nurse</t>
@@ -235,6 +235,9 @@
     <t>Member</t>
   </si>
   <si>
+    <t>Center for the Ecology of Infectious Diseases (CEID)</t>
+  </si>
+  <si>
     <t xml:space="preserve">Eta Sigma Gamma (ESG) | Health Science Honor Society </t>
   </si>
   <si>
@@ -242,6 +245,9 @@
   </si>
   <si>
     <t>Council of State and Territorial Epidemiologists (CSTE)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Present </t>
   </si>
   <si>
     <t>Name of language</t>
@@ -594,8 +600,8 @@
       <c r="E2" s="4">
         <v>2020.0</v>
       </c>
-      <c r="F2" s="4">
-        <v>2022.0</v>
+      <c r="F2" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="G2" s="6"/>
       <c r="H2" s="4" t="b">
@@ -607,13 +613,13 @@
         <v>8</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="4">
         <v>2018.0</v>
@@ -631,13 +637,13 @@
         <v>8</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" s="4">
         <v>2014.0</v>
@@ -652,25 +658,25 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E6" s="4">
         <v>2021.0</v>
       </c>
-      <c r="F6" s="4">
-        <v>2021.0</v>
+      <c r="F6" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H6" s="4" t="b">
         <v>1</v>
@@ -678,22 +684,22 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E7" s="4">
         <v>2021.0</v>
       </c>
-      <c r="F7" s="4">
-        <v>2021.0</v>
+      <c r="F7" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>24</v>
@@ -704,7 +710,7 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>25</v>
@@ -713,13 +719,13 @@
         <v>10</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="E8" s="4">
         <v>2021.0</v>
       </c>
-      <c r="F8" s="4">
-        <v>2021.0</v>
+      <c r="F8" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="G8" s="5" t="s">
         <v>26</v>
@@ -1006,7 +1012,7 @@
         <v>57</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D23" s="5" t="s">
         <v>58</v>
@@ -1115,8 +1121,8 @@
       <c r="E28" s="4">
         <v>2021.0</v>
       </c>
-      <c r="F28" s="4">
-        <v>2021.0</v>
+      <c r="F28" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="H28" s="4" t="b">
         <v>1</v>
@@ -1134,10 +1140,10 @@
         <v>73</v>
       </c>
       <c r="E29" s="4">
-        <v>2019.0</v>
-      </c>
-      <c r="F29" s="4">
-        <v>2020.0</v>
+        <v>2021.0</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="G29" s="5"/>
       <c r="H29" s="4" t="b">
@@ -1151,14 +1157,15 @@
       <c r="B30" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="C30" s="5"/>
+      <c r="D30" s="4" t="s">
         <v>74</v>
       </c>
       <c r="E30" s="4">
         <v>2019.0</v>
       </c>
       <c r="F30" s="4">
-        <v>2021.0</v>
+        <v>2020.0</v>
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="4" t="b">
@@ -1172,15 +1179,14 @@
       <c r="B31" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="4" t="s">
+      <c r="D31" s="5" t="s">
         <v>75</v>
       </c>
       <c r="E31" s="4">
-        <v>2021.0</v>
-      </c>
-      <c r="F31" s="4">
-        <v>2021.0</v>
+        <v>2019.0</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="G31" s="5"/>
       <c r="H31" s="4" t="b">
@@ -1188,14 +1194,26 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="4"/>
-      <c r="B32" s="5"/>
+      <c r="A32" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>72</v>
+      </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
+      <c r="D32" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="E32" s="4">
+        <v>2021.0</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="G32" s="5"/>
-      <c r="H32" s="4"/>
+      <c r="H32" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="4"/>
@@ -1248,9 +1266,14 @@
       <c r="H37" s="4"/>
     </row>
     <row r="38">
+      <c r="A38" s="4"/>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
       <c r="G38" s="5"/>
+      <c r="H38" s="4"/>
     </row>
     <row r="39">
       <c r="B39" s="5"/>
@@ -1465,12 +1488,12 @@
     <row r="81">
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
-      <c r="G81" s="8"/>
+      <c r="G81" s="5"/>
     </row>
     <row r="82">
-      <c r="B82" s="9"/>
-      <c r="C82" s="9"/>
-      <c r="G82" s="9"/>
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="G82" s="8"/>
     </row>
     <row r="83">
       <c r="B83" s="9"/>
@@ -6231,6 +6254,11 @@
       <c r="B1034" s="9"/>
       <c r="C1034" s="9"/>
       <c r="G1034" s="9"/>
+    </row>
+    <row r="1035">
+      <c r="B1035" s="9"/>
+      <c r="C1035" s="9"/>
+      <c r="G1035" s="9"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -6253,10 +6281,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="10" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C1" s="11"/>
       <c r="D1" s="11"/>
@@ -6285,10 +6313,10 @@
     </row>
     <row r="2">
       <c r="A2" s="12" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -6317,7 +6345,7 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B3" s="4">
         <v>5.0</v>
@@ -6325,7 +6353,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B4" s="4">
         <v>4.5</v>
@@ -6333,7 +6361,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B5" s="4">
         <v>4.0</v>
@@ -6341,7 +6369,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B6" s="4">
         <v>4.0</v>
@@ -6349,7 +6377,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B7" s="4">
         <v>3.5</v>
@@ -6357,7 +6385,7 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B8" s="4">
         <v>3.0</v>
@@ -6365,7 +6393,7 @@
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B9" s="4">
         <v>3.0</v>
@@ -6392,10 +6420,10 @@
   <sheetData>
     <row r="1" ht="33.0" customHeight="1">
       <c r="A1" s="14" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
@@ -6427,7 +6455,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -6456,34 +6484,34 @@
     </row>
     <row r="3">
       <c r="A3" s="17" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7">
@@ -9492,13 +9520,13 @@
   <sheetData>
     <row r="1" ht="36.75" customHeight="1">
       <c r="A1" s="14" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
@@ -9530,65 +9558,65 @@
         <v>2</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C5" s="18" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>